<commit_message>
Retirando os comentários antigos
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -1,32 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Insper\Semestre 2\Ciência dos Dados\Projetos\Spotify-Clustering\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
   <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
     <t>Nome Completo</t>
   </si>
   <si>
-    <t>Link da sua playlist favorita do Spotify</t>
-  </si>
-  <si>
     <t>danceability</t>
   </si>
   <si>
@@ -54,6 +49,81 @@
     <t>liveness</t>
   </si>
   <si>
+    <t>11/7/2017 15:03:28</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:06:29</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:17:47</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:20:46</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:21:31</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:21:45</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:22:11</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:22:45</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:24:19</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:28:36</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:29:33</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:31:34</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:32:36</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:37:08</t>
+  </si>
+  <si>
+    <t>11/7/2017 15:55:06</t>
+  </si>
+  <si>
+    <t>11/7/2017 16:01:21</t>
+  </si>
+  <si>
+    <t>11/7/2017 16:07:06</t>
+  </si>
+  <si>
+    <t>11/7/2017 17:12:54</t>
+  </si>
+  <si>
+    <t>11/7/2017 17:39:56</t>
+  </si>
+  <si>
+    <t>11/7/2017 18:04:14</t>
+  </si>
+  <si>
+    <t>11/7/2017 18:29:10</t>
+  </si>
+  <si>
+    <t>11/7/2017 18:37:57</t>
+  </si>
+  <si>
+    <t>11/7/2017 23:01:51</t>
+  </si>
+  <si>
+    <t>11/8/2017 8:54:17</t>
+  </si>
+  <si>
+    <t>11/8/2017 9:50:05</t>
+  </si>
+  <si>
     <t>David Fogelman</t>
   </si>
   <si>
@@ -127,81 +197,6 @@
   </si>
   <si>
     <t>Matteo Iannoni</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/david.fogelman/playlist/1XWEEUIToeZVyEr1eICAdY?si=AiJxoBQYRwmLtH8pXneFCQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12159396059/playlist/20s68w1KUNG1h4W7LpGuWY</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/222q2mlkcu5l53rgcr3l3mb3y/playlist/5re8yP7xnbVeWD8KgcFLTd</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/luca_salimon/playlist/0u1ErOb0FkLAFT7tG01kKr</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12164789732/playlist/2sfcCsbeJQZ0OubjEWaMgl?si=hbV8YCKwR8Gg5qTCtWygRA</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/p1e2d3r4o5/playlist/77bVYMzIafJxcanc7081XX?si=eIJQBFRYTae6HZc0zunwgA</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/guimamone/playlist/3eazNmWsI8BjLT0KUMV2v7?si=I7PoVqTkSae6bWoA64R3bw</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/hugogloss/playlist/2ZD2ZMLJWTcsOqEIiLGRuE?si=Zcs8WiRYQ4W0SqHIRywNTg</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/paulo_gan/playlist/3Gl5Lp6r65ph633tkaKSGk?si=wTHl3G6wQ6OtuSx5hVJLvw</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/gpizzigh/playlist/07LMxF1kj7ATRA5zHsvEED</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/spotify/playlist/37i9dQZF1DXdSjVZQzv2tl?si=pOhtZj0iSZeCkrQK3NOaQQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/22be5rdyh3buhqccqdauevzui/playlist/3eFFXYaOtwAdUOaRt0CTvL</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/spotify/playlist/37i9dQZF1DWYBO1MoTDhZI?si=iWvLbL-cRea2bCpqsy38ZQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12167935604/playlist/7sF2NaA2UvgiIvk9baPuJo</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/chicarelle/playlist/1iFzfr4CxjDdz0KTMot9LX?si=MNlCv4atSK6NBCxCERGHGQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/amonglies/playlist/2GlwkxTcNsbBDAiukvCOQ3?si=xFSbNqpwRRqNZhC-scJKlA</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/spotify/playlist/37i9dQZF1DX7KTVQYEg01L?si=FUWglHbYRUCj43d488V2fw</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/v_botteon/playlist/577A42XE1of1ytmM0TxoDo?si=248VF39dSKSEpw0Y0LHf2g</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12154657301/playlist/6pmTsaQCPPWBbijDeQR9dS?si=tnIowQT5</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12154657301/playlist/12Er0EmzXHh41LBluaDqNK</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/hurtbyspectre/playlist/5D0Tyj4ybsyHIrb6x0gphz?si=LQDjYc_FQGqRyNaamNXCeQ</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/227lbfuksgn3mon42vghtx5uy/playlist/6zxDqmSa3CmpamVV1fbowu</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/mopiik/playlist/5vwzvKpgATpSkRXzaJfcpC</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/12168025855/playlist/09UxJWqbe0StBDhDTCOHHe?si=N_S-_3H5Rq6zBWAFP7EpgA</t>
-  </si>
-  <si>
-    <t>https://open.spotify.com/user/spotify/playlist/37i9dQZF1DXdPec7aLTmlC?si=gRt6jfjGRNyTCIi-GhXR4w</t>
   </si>
   <si>
     <t>0.7237916666666666</t>
@@ -882,8 +877,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,14 +890,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -943,26 +930,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1009,7 +987,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1041,27 +1019,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,24 +1053,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1286,20 +1228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,14 +1270,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
@@ -1372,14 +1308,14 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
       <c r="D3" t="s">
@@ -1410,14 +1346,14 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
@@ -1448,14 +1384,14 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
@@ -1486,14 +1422,14 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
@@ -1524,14 +1460,14 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
       <c r="D7" t="s">
@@ -1562,14 +1498,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
       <c r="D8" t="s">
@@ -1600,14 +1536,14 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
       <c r="D9" t="s">
@@ -1638,14 +1574,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
@@ -1676,14 +1612,14 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
       <c r="D11" t="s">
@@ -1714,14 +1650,14 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
@@ -1752,14 +1688,14 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
       <c r="D13" t="s">
@@ -1790,14 +1726,14 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>48</v>
       </c>
       <c r="D14" t="s">
@@ -1828,14 +1764,14 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>49</v>
       </c>
       <c r="D15" t="s">
@@ -1866,14 +1802,14 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
       <c r="D16" t="s">
@@ -1904,14 +1840,14 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>51</v>
       </c>
       <c r="D17" t="s">
@@ -1942,14 +1878,14 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="D18" t="s">
@@ -1980,14 +1916,14 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>53</v>
       </c>
       <c r="D19" t="s">
@@ -2018,14 +1954,14 @@
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>54</v>
       </c>
       <c r="D20" t="s">
@@ -2056,14 +1992,14 @@
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>55</v>
       </c>
       <c r="D21" t="s">
@@ -2094,14 +2030,14 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>56</v>
       </c>
       <c r="D22" t="s">
@@ -2132,14 +2068,14 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>57</v>
       </c>
       <c r="D23" t="s">
@@ -2170,14 +2106,14 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>58</v>
       </c>
       <c r="D24" t="s">
@@ -2208,14 +2144,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>59</v>
       </c>
       <c r="D25" t="s">
@@ -2246,14 +2182,14 @@
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
@@ -2285,33 +2221,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inicio etapa de PCA
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
-  <si>
-    <t>Timestamp</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="280">
   <si>
     <t>Nome Completo</t>
   </si>
@@ -49,85 +46,10 @@
     <t>liveness</t>
   </si>
   <si>
-    <t>11/7/2017 15:03:28</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:06:29</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:17:47</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:20:46</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:21:31</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:21:45</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:22:11</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:22:45</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:24:19</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:28:36</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:29:33</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:31:34</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:32:36</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:37:08</t>
-  </si>
-  <si>
-    <t>11/7/2017 15:55:06</t>
-  </si>
-  <si>
-    <t>11/7/2017 16:01:21</t>
-  </si>
-  <si>
-    <t>11/7/2017 16:07:06</t>
-  </si>
-  <si>
-    <t>11/7/2017 17:12:54</t>
-  </si>
-  <si>
-    <t>11/7/2017 17:39:56</t>
-  </si>
-  <si>
-    <t>11/7/2017 18:04:14</t>
-  </si>
-  <si>
-    <t>11/7/2017 18:29:10</t>
-  </si>
-  <si>
-    <t>11/7/2017 18:37:57</t>
-  </si>
-  <si>
-    <t>11/7/2017 23:01:51</t>
-  </si>
-  <si>
-    <t>11/8/2017 8:54:17</t>
-  </si>
-  <si>
-    <t>11/8/2017 9:50:05</t>
-  </si>
-  <si>
     <t>David Fogelman</t>
   </si>
   <si>
-    <t>Wesley Gabriel Albano da Silva</t>
+    <t>Wesley Gabriel Albano Da Silva</t>
   </si>
   <si>
     <t>André Neustein</t>
@@ -136,13 +58,13 @@
     <t>Luca Salimon Nascimento</t>
   </si>
   <si>
-    <t>Manoela Cirne lima de campos</t>
+    <t>Manoela Cirne Lima De Campos</t>
   </si>
   <si>
     <t>Pedro Villas Boas Dias</t>
   </si>
   <si>
-    <t>Rodrigo coutinho</t>
+    <t>Rodrigo Coutinho</t>
   </si>
   <si>
     <t>Emanuelle Moço</t>
@@ -151,7 +73,7 @@
     <t xml:space="preserve">Giovana Lemes </t>
   </si>
   <si>
-    <t xml:space="preserve">gabriel pizzighini salvador </t>
+    <t xml:space="preserve">Gabriel Pizzighini Salvador </t>
   </si>
   <si>
     <t>Luca Ribeiro Noto</t>
@@ -160,7 +82,7 @@
     <t>Pedro Cunial</t>
   </si>
   <si>
-    <t>Luigi crespi corradi</t>
+    <t>Luigi Crespi Corradi</t>
   </si>
   <si>
     <t>Iago Rainha Mendes</t>
@@ -169,13 +91,13 @@
     <t>Guilherme Benavente Chicarelle</t>
   </si>
   <si>
-    <t>Bruna D'Urso de Oliveira</t>
+    <t>Bruna D'Urso De Oliveira</t>
   </si>
   <si>
     <t>Natália De Munno Farah</t>
   </si>
   <si>
-    <t>Lucas Sozzi de Jesus</t>
+    <t>Lucas Sozzi De Jesus</t>
   </si>
   <si>
     <t>Juliana Costa Pessoa</t>
@@ -199,6 +121,12 @@
     <t>Matteo Iannoni</t>
   </si>
   <si>
+    <t>Guilherme Leite</t>
+  </si>
+  <si>
+    <t>Roberta Thome</t>
+  </si>
+  <si>
     <t>0.7237916666666666</t>
   </si>
   <si>
@@ -223,7 +151,7 @@
     <t>0.6739299999999999</t>
   </si>
   <si>
-    <t>0.8114199999999998</t>
+    <t>0.8125299999999998</t>
   </si>
   <si>
     <t>0.6701506849315068</t>
@@ -235,7 +163,7 @@
     <t>0.4847638888888889</t>
   </si>
   <si>
-    <t>0.6604266666666665</t>
+    <t>0.6589466666666669</t>
   </si>
   <si>
     <t>0.43084000000000006</t>
@@ -274,6 +202,12 @@
     <t>0.6936458333333332</t>
   </si>
   <si>
+    <t>0.45916</t>
+  </si>
+  <si>
+    <t>0.6980799999999998</t>
+  </si>
+  <si>
     <t>0.7855625</t>
   </si>
   <si>
@@ -298,7 +232,7 @@
     <t>0.6741400000000002</t>
   </si>
   <si>
-    <t>0.6121099999999999</t>
+    <t>0.6101899999999999</t>
   </si>
   <si>
     <t>0.7475753424657532</t>
@@ -310,7 +244,7 @@
     <t>0.9001666666666667</t>
   </si>
   <si>
-    <t>0.6810666666666666</t>
+    <t>0.6803866666666665</t>
   </si>
   <si>
     <t>0.9445699999999999</t>
@@ -349,6 +283,12 @@
     <t>0.7176458333333332</t>
   </si>
   <si>
+    <t>0.8227599999999999</t>
+  </si>
+  <si>
+    <t>0.70351</t>
+  </si>
+  <si>
     <t>0.07103124999999999</t>
   </si>
   <si>
@@ -373,7 +313,7 @@
     <t>0.093297</t>
   </si>
   <si>
-    <t>0.17330600000000002</t>
+    <t>0.17505000000000004</t>
   </si>
   <si>
     <t>0.15366301369863014</t>
@@ -385,7 +325,7 @@
     <t>0.0827361111111111</t>
   </si>
   <si>
-    <t>0.08914133333333335</t>
+    <t>0.09467333333333336</t>
   </si>
   <si>
     <t>0.10666900000000004</t>
@@ -424,6 +364,12 @@
     <t>0.06907291666666666</t>
   </si>
   <si>
+    <t>0.07062799999999998</t>
+  </si>
+  <si>
+    <t>0.102141</t>
+  </si>
+  <si>
     <t>0.07960545833333334</t>
   </si>
   <si>
@@ -448,7 +394,7 @@
     <t>0.14503371999999992</t>
   </si>
   <si>
-    <t>0.2821757000000001</t>
+    <t>0.2867107000000001</t>
   </si>
   <si>
     <t>0.17852123287671232</t>
@@ -460,7 +406,7 @@
     <t>0.022618597222222217</t>
   </si>
   <si>
-    <t>0.18789462666666668</t>
+    <t>0.18760262666666663</t>
   </si>
   <si>
     <t>0.004553164500000003</t>
@@ -499,6 +445,12 @@
     <t>0.13918447916666668</t>
   </si>
   <si>
+    <t>0.047298245</t>
+  </si>
+  <si>
+    <t>0.24518014999999987</t>
+  </si>
+  <si>
     <t>0.04932250208333336</t>
   </si>
   <si>
@@ -523,7 +475,7 @@
     <t>0.004264186599999999</t>
   </si>
   <si>
-    <t>0.0026383783</t>
+    <t>0.0026332133999999994</t>
   </si>
   <si>
     <t>0.0007574817808219177</t>
@@ -535,7 +487,7 @@
     <t>0.008256855833333332</t>
   </si>
   <si>
-    <t>0.03050780653333333</t>
+    <t>0.029048073199999996</t>
   </si>
   <si>
     <t>0.0134167286</t>
@@ -574,6 +526,12 @@
     <t>0.006573627083333332</t>
   </si>
   <si>
+    <t>0.029207116200000015</t>
+  </si>
+  <si>
+    <t>0.020180939599999993</t>
+  </si>
+  <si>
     <t>0.48941666666666667</t>
   </si>
   <si>
@@ -598,7 +556,7 @@
     <t>0.5137180000000001</t>
   </si>
   <si>
-    <t>0.6363399999999998</t>
+    <t>0.6332599999999998</t>
   </si>
   <si>
     <t>0.5403123287671234</t>
@@ -610,7 +568,7 @@
     <t>0.5590555555555556</t>
   </si>
   <si>
-    <t>0.4620573333333333</t>
+    <t>0.4645773333333331</t>
   </si>
   <si>
     <t>0.3835059999999999</t>
@@ -649,6 +607,12 @@
     <t>0.5339375000000001</t>
   </si>
   <si>
+    <t>0.523129</t>
+  </si>
+  <si>
+    <t>0.56718</t>
+  </si>
+  <si>
     <t>-5.365875000000002</t>
   </si>
   <si>
@@ -673,7 +637,7 @@
     <t>-5.477929999999999</t>
   </si>
   <si>
-    <t>-3.4437200000000012</t>
+    <t>-3.4802000000000004</t>
   </si>
   <si>
     <t>-5.904150684931506</t>
@@ -685,7 +649,7 @@
     <t>-4.728152777777778</t>
   </si>
   <si>
-    <t>-5.886586666666664</t>
+    <t>-5.95128</t>
   </si>
   <si>
     <t>-3.7509699999999992</t>
@@ -724,6 +688,12 @@
     <t>-5.22175</t>
   </si>
   <si>
+    <t>-6.54646</t>
+  </si>
+  <si>
+    <t>-4.91393</t>
+  </si>
+  <si>
     <t>122.18829166666666</t>
   </si>
   <si>
@@ -748,7 +718,7 @@
     <t>119.66069999999999</t>
   </si>
   <si>
-    <t>121.60030000000002</t>
+    <t>121.14699000000002</t>
   </si>
   <si>
     <t>117.27619178082192</t>
@@ -760,7 +730,7 @@
     <t>131.44608333333335</t>
   </si>
   <si>
-    <t>113.07325333333334</t>
+    <t>113.71114666666668</t>
   </si>
   <si>
     <t>128.63044000000002</t>
@@ -799,6 +769,12 @@
     <t>110.87124999999997</t>
   </si>
   <si>
+    <t>131.65472999999994</t>
+  </si>
+  <si>
+    <t>123.19328999999999</t>
+  </si>
+  <si>
     <t>0.22062916666666674</t>
   </si>
   <si>
@@ -823,7 +799,7 @@
     <t>0.15602999999999997</t>
   </si>
   <si>
-    <t>0.147293</t>
+    <t>0.14753700000000003</t>
   </si>
   <si>
     <t>0.21163424657534252</t>
@@ -835,7 +811,7 @@
     <t>0.26920416666666663</t>
   </si>
   <si>
-    <t>0.1566346666666667</t>
+    <t>0.15626399999999993</t>
   </si>
   <si>
     <t>0.266119</t>
@@ -872,6 +848,12 @@
   </si>
   <si>
     <t>0.17288333333333336</t>
+  </si>
+  <si>
+    <t>0.29741600000000007</t>
+  </si>
+  <si>
+    <t>0.283656</t>
   </si>
 </sst>
 </file>
@@ -1229,13 +1211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,958 +1248,950 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="G2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I2" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="J2" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="K2" t="s">
-        <v>236</v>
-      </c>
-      <c r="L2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="G3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="J3" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="K3" t="s">
-        <v>237</v>
-      </c>
-      <c r="L3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G4" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="H4" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="J4" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="K4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="I5" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="K5" t="s">
-        <v>239</v>
-      </c>
-      <c r="L5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="H6" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="J6" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="K6" t="s">
-        <v>240</v>
-      </c>
-      <c r="L6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="H7" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="I7" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="J7" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="K7" t="s">
-        <v>241</v>
-      </c>
-      <c r="L7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="H8" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="I8" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="J8" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="K8" t="s">
-        <v>242</v>
-      </c>
-      <c r="L8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="H9" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="I9" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="J9" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="K9" t="s">
-        <v>243</v>
-      </c>
-      <c r="L9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="I10" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="J10" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="K10" t="s">
-        <v>244</v>
-      </c>
-      <c r="L10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="H11" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="I11" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="J11" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="K11" t="s">
-        <v>245</v>
-      </c>
-      <c r="L11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="G12" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="H12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="I12" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="J12" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="K12" t="s">
-        <v>246</v>
-      </c>
-      <c r="L12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G13" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="H13" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="I13" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="J13" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="K13" t="s">
-        <v>247</v>
-      </c>
-      <c r="L13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="G14" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="H14" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="I14" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="J14" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="K14" t="s">
-        <v>248</v>
-      </c>
-      <c r="L14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G15" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="I15" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="J15" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="K15" t="s">
-        <v>249</v>
-      </c>
-      <c r="L15" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G16" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="H16" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="I16" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="J16" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="K16" t="s">
-        <v>250</v>
-      </c>
-      <c r="L16" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="H17" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="I17" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="J17" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="K17" t="s">
-        <v>251</v>
-      </c>
-      <c r="L17" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H18" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I18" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="J18" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="K18" t="s">
-        <v>252</v>
-      </c>
-      <c r="L18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="H19" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="I19" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="J19" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="K19" t="s">
-        <v>253</v>
-      </c>
-      <c r="L19" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G20" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="H20" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="I20" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="J20" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="K20" t="s">
-        <v>254</v>
-      </c>
-      <c r="L20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="G21" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="H21" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="J21" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="K21" t="s">
-        <v>255</v>
-      </c>
-      <c r="L21" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="G22" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="H22" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="J22" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="K22" t="s">
-        <v>256</v>
-      </c>
-      <c r="L22" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="G23" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="H23" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="I23" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="J23" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="K23" t="s">
-        <v>257</v>
-      </c>
-      <c r="L23" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="H24" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I24" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="J24" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="K24" t="s">
-        <v>258</v>
-      </c>
-      <c r="L24" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="G25" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="I25" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="J25" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="K25" t="s">
-        <v>259</v>
-      </c>
-      <c r="L25" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" t="s">
+        <v>223</v>
+      </c>
+      <c r="J26" t="s">
+        <v>250</v>
+      </c>
+      <c r="K26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" t="s">
-        <v>160</v>
-      </c>
-      <c r="H26" t="s">
-        <v>185</v>
-      </c>
-      <c r="I26" t="s">
-        <v>210</v>
-      </c>
-      <c r="J26" t="s">
-        <v>235</v>
-      </c>
-      <c r="K26" t="s">
-        <v>260</v>
-      </c>
-      <c r="L26" t="s">
-        <v>285</v>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" t="s">
+        <v>170</v>
+      </c>
+      <c r="H27" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" t="s">
+        <v>224</v>
+      </c>
+      <c r="J27" t="s">
+        <v>251</v>
+      </c>
+      <c r="K27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>171</v>
+      </c>
+      <c r="H28" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28" t="s">
+        <v>225</v>
+      </c>
+      <c r="J28" t="s">
+        <v>252</v>
+      </c>
+      <c r="K28" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checa se os valores foram já calculados
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="280">
-  <si>
-    <t>Nome Completo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
   <si>
     <t>danceability</t>
   </si>
@@ -44,87 +41,6 @@
   </si>
   <si>
     <t>liveness</t>
-  </si>
-  <si>
-    <t>David Fogelman</t>
-  </si>
-  <si>
-    <t>Wesley Gabriel Albano Da Silva</t>
-  </si>
-  <si>
-    <t>André Neustein</t>
-  </si>
-  <si>
-    <t>Luca Salimon Nascimento</t>
-  </si>
-  <si>
-    <t>Manoela Cirne Lima De Campos</t>
-  </si>
-  <si>
-    <t>Pedro Villas Boas Dias</t>
-  </si>
-  <si>
-    <t>Rodrigo Coutinho</t>
-  </si>
-  <si>
-    <t>Emanuelle Moço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giovana Lemes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabriel Pizzighini Salvador </t>
-  </si>
-  <si>
-    <t>Luca Ribeiro Noto</t>
-  </si>
-  <si>
-    <t>Pedro Cunial</t>
-  </si>
-  <si>
-    <t>Luigi Crespi Corradi</t>
-  </si>
-  <si>
-    <t>Iago Rainha Mendes</t>
-  </si>
-  <si>
-    <t>Guilherme Benavente Chicarelle</t>
-  </si>
-  <si>
-    <t>Bruna D'Urso De Oliveira</t>
-  </si>
-  <si>
-    <t>Natália De Munno Farah</t>
-  </si>
-  <si>
-    <t>Lucas Sozzi De Jesus</t>
-  </si>
-  <si>
-    <t>Juliana Costa Pessoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana Capriles </t>
-  </si>
-  <si>
-    <t>Barbara Freire</t>
-  </si>
-  <si>
-    <t>Lucas Chen Alba</t>
-  </si>
-  <si>
-    <t>Bruno Arthur Cesconetto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">João Gabriel Rodrigues Edivirges </t>
-  </si>
-  <si>
-    <t>Matteo Iannoni</t>
-  </si>
-  <si>
-    <t>Guilherme Leite</t>
-  </si>
-  <si>
-    <t>Roberta Thome</t>
   </si>
   <si>
     <t>0.7237916666666666</t>
@@ -1211,13 +1127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,953 +1161,869 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J2" t="s">
-        <v>226</v>
-      </c>
-      <c r="K2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J3" t="s">
-        <v>227</v>
-      </c>
-      <c r="K3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J4" t="s">
-        <v>228</v>
-      </c>
-      <c r="K4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J5" t="s">
-        <v>229</v>
-      </c>
-      <c r="K5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J6" t="s">
-        <v>230</v>
-      </c>
-      <c r="K6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J7" t="s">
-        <v>231</v>
-      </c>
-      <c r="K7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J8" t="s">
-        <v>232</v>
-      </c>
-      <c r="K8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9" t="s">
-        <v>233</v>
-      </c>
-      <c r="K9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10" t="s">
-        <v>234</v>
-      </c>
-      <c r="K10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J11" t="s">
-        <v>235</v>
-      </c>
-      <c r="K11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J12" t="s">
-        <v>236</v>
-      </c>
-      <c r="K12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J13" t="s">
-        <v>237</v>
-      </c>
-      <c r="K13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J14" t="s">
-        <v>238</v>
-      </c>
-      <c r="K14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J15" t="s">
-        <v>239</v>
-      </c>
-      <c r="K15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J16" t="s">
-        <v>240</v>
-      </c>
-      <c r="K16" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J17" t="s">
-        <v>241</v>
-      </c>
-      <c r="K17" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J18" t="s">
-        <v>242</v>
-      </c>
-      <c r="K18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J19" t="s">
-        <v>243</v>
-      </c>
-      <c r="K19" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J20" t="s">
-        <v>244</v>
-      </c>
-      <c r="K20" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J21" t="s">
-        <v>245</v>
-      </c>
-      <c r="K21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J22" t="s">
-        <v>246</v>
-      </c>
-      <c r="K22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J23" t="s">
-        <v>247</v>
-      </c>
-      <c r="K23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J24" t="s">
-        <v>248</v>
-      </c>
-      <c r="K24" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J25" t="s">
-        <v>249</v>
-      </c>
-      <c r="K25" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J26" t="s">
-        <v>250</v>
-      </c>
-      <c r="K26" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J27" t="s">
-        <v>251</v>
-      </c>
-      <c r="K27" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J28" t="s">
-        <v>252</v>
-      </c>
-      <c r="K28" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adionamos o sheets e começamos a análise de pessoas
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,31 +438,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.7237916667000001</v>
+        <v>0.5350240598391367</v>
       </c>
       <c r="C2">
-        <v>0.7855625000000001</v>
+        <v>0.358529043345658</v>
       </c>
       <c r="D2">
-        <v>0.07103125</v>
+        <v>-0.8066088955090872</v>
       </c>
       <c r="E2">
-        <v>0.07960545832999999</v>
+        <v>-0.7125982158326621</v>
       </c>
       <c r="F2">
-        <v>0.04932250208</v>
+        <v>-0.8742797670534763</v>
       </c>
       <c r="G2">
-        <v>0.4894166667</v>
+        <v>-0.2127763180785625</v>
       </c>
       <c r="H2">
-        <v>-5.365875</v>
+        <v>0.5825506654107084</v>
       </c>
       <c r="I2">
-        <v>122.1882917</v>
+        <v>-0.2289264902670407</v>
       </c>
       <c r="J2">
-        <v>0.2206291667</v>
+        <v>-0.5448451679015014</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -470,31 +470,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5287882353</v>
+        <v>-0.4867655149466845</v>
       </c>
       <c r="C3">
-        <v>0.7707176470999999</v>
+        <v>0.2986416670196603</v>
       </c>
       <c r="D3">
-        <v>0.06866235294</v>
+        <v>-0.8299929888598778</v>
       </c>
       <c r="E3">
-        <v>0.06516938235</v>
+        <v>-0.7678790577803445</v>
       </c>
       <c r="F3">
-        <v>0.02695773729</v>
+        <v>-0.9313140240909471</v>
       </c>
       <c r="G3">
-        <v>0.4570258824</v>
+        <v>-0.3577796777975779</v>
       </c>
       <c r="H3">
-        <v>-5.629929412</v>
+        <v>0.5240944952940305</v>
       </c>
       <c r="I3">
-        <v>124.3847412</v>
+        <v>-0.07927395121912006</v>
       </c>
       <c r="J3">
-        <v>0.2329682353</v>
+        <v>-0.4680081147609649</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -502,31 +502,31 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7438</v>
+        <v>0.6398648117582333</v>
       </c>
       <c r="C4">
-        <v>0.73441</v>
+        <v>0.1521686948698862</v>
       </c>
       <c r="D4">
-        <v>0.240146</v>
+        <v>0.8627735220602153</v>
       </c>
       <c r="E4">
-        <v>0.1840844</v>
+        <v>-0.3125113868825971</v>
       </c>
       <c r="F4">
-        <v>0.0016399424</v>
+        <v>-0.9958790501458545</v>
       </c>
       <c r="G4">
-        <v>0.655183</v>
+        <v>0.5293074497665442</v>
       </c>
       <c r="H4">
-        <v>-5.71197</v>
+        <v>0.5059324106983742</v>
       </c>
       <c r="I4">
-        <v>111.13596</v>
+        <v>-0.9819642911838509</v>
       </c>
       <c r="J4">
-        <v>0.215125</v>
+        <v>-0.5791203602140129</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -534,31 +534,31 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.4884021739</v>
+        <v>-0.698382593727894</v>
       </c>
       <c r="C5">
-        <v>0.8203478261</v>
+        <v>0.4988606403514608</v>
       </c>
       <c r="D5">
-        <v>0.1431304348</v>
+        <v>-0.09489621860657027</v>
       </c>
       <c r="E5">
-        <v>0.4735684783</v>
+        <v>0.7960255591021403</v>
       </c>
       <c r="F5">
-        <v>2.4e-05</v>
+        <v>-0.9999999999999999</v>
       </c>
       <c r="G5">
-        <v>0.760326087</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="H5">
-        <v>-5.73526087</v>
+        <v>0.5007762951516836</v>
       </c>
       <c r="I5">
-        <v>140.2252391</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0.4687119565</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -566,31 +566,31 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.6044583333</v>
+        <v>-0.09026522413476901</v>
       </c>
       <c r="C6">
-        <v>0.4997888889</v>
+        <v>-0.7943440708085987</v>
       </c>
       <c r="D6">
-        <v>0.07998194444000001</v>
+        <v>-0.7182539062300839</v>
       </c>
       <c r="E6">
-        <v>0.5232716667</v>
+        <v>0.9863566508782506</v>
       </c>
       <c r="F6">
-        <v>0.007501033472</v>
+        <v>-0.9809321916450245</v>
       </c>
       <c r="G6">
-        <v>0.6309166667</v>
+        <v>0.4206747033664699</v>
       </c>
       <c r="H6">
-        <v>-11.79668056</v>
+        <v>-0.8410963055122327</v>
       </c>
       <c r="I6">
-        <v>119.781</v>
+        <v>-0.3929445180587052</v>
       </c>
       <c r="J6">
-        <v>0.2760361111</v>
+        <v>-0.1998186128811694</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -598,31 +598,31 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.51615</v>
+        <v>-0.5529880269328511</v>
       </c>
       <c r="C7">
-        <v>0.75121</v>
+        <v>0.219943561286835</v>
       </c>
       <c r="D7">
-        <v>0.05461900000000001</v>
+        <v>-0.9686191375651573</v>
       </c>
       <c r="E7">
-        <v>0.085612374</v>
+        <v>-0.6895956106782989</v>
       </c>
       <c r="F7">
-        <v>0.0413066502</v>
+        <v>-0.8947216612916233</v>
       </c>
       <c r="G7">
-        <v>0.46897</v>
+        <v>-0.3043096177694538</v>
       </c>
       <c r="H7">
-        <v>-6.67714</v>
+        <v>0.292263791097676</v>
       </c>
       <c r="I7">
-        <v>119.50044</v>
+        <v>-0.4120601482406361</v>
       </c>
       <c r="J7">
-        <v>0.177666</v>
+        <v>-0.8123826320188197</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -630,31 +630,31 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.63284</v>
+        <v>0.05845057507401297</v>
       </c>
       <c r="C8">
-        <v>0.73042</v>
+        <v>0.1360721640958609</v>
       </c>
       <c r="D8">
-        <v>0.067093</v>
+        <v>-0.8454845424056017</v>
       </c>
       <c r="E8">
-        <v>0.1424736</v>
+        <v>-0.4718538606478692</v>
       </c>
       <c r="F8">
-        <v>0.0115342393</v>
+        <v>-0.9706467761694265</v>
       </c>
       <c r="G8">
-        <v>0.470034</v>
+        <v>-0.2995464242230401</v>
       </c>
       <c r="H8">
-        <v>-5.63649</v>
+        <v>0.5226421171826834</v>
       </c>
       <c r="I8">
-        <v>120.20743</v>
+        <v>-0.3638902046195831</v>
       </c>
       <c r="J8">
-        <v>0.168138</v>
+        <v>-0.8717147798539515</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -662,31 +662,31 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.67393</v>
+        <v>0.2737561895779299</v>
       </c>
       <c r="C9">
-        <v>0.67414</v>
+        <v>-0.09097363840091699</v>
       </c>
       <c r="D9">
-        <v>0.093297</v>
+        <v>-0.5868169993912519</v>
       </c>
       <c r="E9">
-        <v>0.14503372</v>
+        <v>-0.4620502554795968</v>
       </c>
       <c r="F9">
-        <v>0.0042641866</v>
+        <v>-0.9891867455480966</v>
       </c>
       <c r="G9">
-        <v>0.513718</v>
+        <v>-0.1039868876802501</v>
       </c>
       <c r="H9">
-        <v>-5.477930000000001</v>
+        <v>0.557744012521211</v>
       </c>
       <c r="I9">
-        <v>119.6607</v>
+        <v>-0.4011410190242248</v>
       </c>
       <c r="J9">
-        <v>0.15603</v>
+        <v>-0.9471129374933066</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -694,31 +694,31 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.81253</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.61019</v>
+        <v>-0.3489618947916227</v>
       </c>
       <c r="D10">
-        <v>0.17505</v>
+        <v>0.2201913826898096</v>
       </c>
       <c r="E10">
-        <v>0.2867107</v>
+        <v>0.08048102170788751</v>
       </c>
       <c r="F10">
-        <v>0.0026332134</v>
+        <v>-0.9933460267023352</v>
       </c>
       <c r="G10">
-        <v>0.63326</v>
+        <v>0.4311650699563723</v>
       </c>
       <c r="H10">
-        <v>-3.4802</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>121.14699</v>
+        <v>-0.2998743738035934</v>
       </c>
       <c r="J10">
-        <v>0.147537</v>
+        <v>-0.9999999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -726,31 +726,31 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.6701506849000001</v>
+        <v>0.2539531289790147</v>
       </c>
       <c r="C11">
-        <v>0.7475753425</v>
+        <v>0.2052805597074383</v>
       </c>
       <c r="D11">
-        <v>0.1536630137</v>
+        <v>0.009074026610487396</v>
       </c>
       <c r="E11">
-        <v>0.1785212329</v>
+        <v>-0.3338147217784313</v>
       </c>
       <c r="F11">
-        <v>0.0007574817808</v>
+        <v>-0.9981294867703167</v>
       </c>
       <c r="G11">
-        <v>0.5403123288</v>
+        <v>0.01506756280035093</v>
       </c>
       <c r="H11">
-        <v>-5.904150685</v>
+        <v>0.4633875930207976</v>
       </c>
       <c r="I11">
-        <v>117.2761918</v>
+        <v>-0.5636067194696883</v>
       </c>
       <c r="J11">
-        <v>0.2116342466</v>
+        <v>-0.6008577549227441</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -758,31 +758,31 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.64066</v>
+        <v>0.0994262359506406</v>
       </c>
       <c r="C12">
-        <v>0.81684</v>
+        <v>0.4847093043192356</v>
       </c>
       <c r="D12">
-        <v>0.093614</v>
+        <v>-0.5836877973176925</v>
       </c>
       <c r="E12">
-        <v>0.377852</v>
+        <v>0.4294933022740577</v>
       </c>
       <c r="F12">
-        <v>0.0001087476</v>
+        <v>-0.9997838780578694</v>
       </c>
       <c r="G12">
-        <v>0.68492</v>
+        <v>0.6624306513546077</v>
       </c>
       <c r="H12">
-        <v>-4.245</v>
+        <v>0.8306891425649223</v>
       </c>
       <c r="I12">
-        <v>134.46476</v>
+        <v>0.6075164380298848</v>
       </c>
       <c r="J12">
-        <v>0.441344</v>
+        <v>0.8295760242439703</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -790,31 +790,31 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.4847638889</v>
+        <v>-0.7174466771463752</v>
       </c>
       <c r="C13">
-        <v>0.9001666667</v>
+        <v>0.8208672629241223</v>
       </c>
       <c r="D13">
-        <v>0.08273611111000001</v>
+        <v>-0.6910667010102353</v>
       </c>
       <c r="E13">
-        <v>0.02261859722</v>
+        <v>-0.9308210671449506</v>
       </c>
       <c r="F13">
-        <v>0.008256855833000001</v>
+        <v>-0.9790047058334493</v>
       </c>
       <c r="G13">
-        <v>0.5590555556</v>
+        <v>0.0989750975115582</v>
       </c>
       <c r="H13">
-        <v>-4.728152778</v>
+        <v>0.7237291384915439</v>
       </c>
       <c r="I13">
-        <v>131.4460833</v>
+        <v>0.40184240240111</v>
       </c>
       <c r="J13">
-        <v>0.2692041667</v>
+        <v>-0.2423620569557075</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -822,31 +822,31 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.6589466667</v>
+        <v>0.1952457056773822</v>
       </c>
       <c r="C14">
-        <v>0.6803866667</v>
+        <v>-0.06577322166617261</v>
       </c>
       <c r="D14">
-        <v>0.09467333332999998</v>
+        <v>-0.5732308003056217</v>
       </c>
       <c r="E14">
-        <v>0.1876026267</v>
+        <v>-0.2990388522126308</v>
       </c>
       <c r="F14">
-        <v>0.0290480732</v>
+        <v>-0.92598328367382</v>
       </c>
       <c r="G14">
-        <v>0.4645773333</v>
+        <v>-0.3239742058117332</v>
       </c>
       <c r="H14">
-        <v>-5.951280000000001</v>
+        <v>0.4529541401795607</v>
       </c>
       <c r="I14">
-        <v>113.7111467</v>
+        <v>-0.8065069323065188</v>
       </c>
       <c r="J14">
-        <v>0.156264</v>
+        <v>-0.945655787766877</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -854,31 +854,31 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.4308399999999999</v>
+        <v>-1</v>
       </c>
       <c r="C15">
-        <v>0.94457</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.106669</v>
+        <v>-0.4548179769065974</v>
       </c>
       <c r="E15">
-        <v>0.0045531645</v>
+        <v>-1</v>
       </c>
       <c r="F15">
-        <v>0.0134167286</v>
+        <v>-0.9658460827744977</v>
       </c>
       <c r="G15">
-        <v>0.383506</v>
+        <v>-0.6869050813509252</v>
       </c>
       <c r="H15">
-        <v>-3.75097</v>
+        <v>0.9400571379867994</v>
       </c>
       <c r="I15">
-        <v>128.63044</v>
+        <v>0.2100018119854106</v>
       </c>
       <c r="J15">
-        <v>0.266119</v>
+        <v>-0.261573808292864</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -886,31 +886,31 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.6007307692</v>
+        <v>-0.1097971170321461</v>
       </c>
       <c r="C16">
-        <v>0.5036333332999999</v>
+        <v>-0.7788347430908975</v>
       </c>
       <c r="D16">
-        <v>0.05806153846</v>
+        <v>-0.9346368079520981</v>
       </c>
       <c r="E16">
-        <v>0.4719334615</v>
+        <v>0.7897645013584829</v>
       </c>
       <c r="F16">
-        <v>0.04665651449</v>
+        <v>-0.8810785249610379</v>
       </c>
       <c r="G16">
-        <v>0.5695641026</v>
+        <v>0.1460185592151144</v>
       </c>
       <c r="H16">
-        <v>-10.69234615</v>
+        <v>-0.5966195719189265</v>
       </c>
       <c r="I16">
-        <v>115.7571923</v>
+        <v>-0.667101988533477</v>
       </c>
       <c r="J16">
-        <v>0.2339038462</v>
+        <v>-0.4621819388337021</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -918,31 +918,31 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.6078</v>
+        <v>-0.07275537740050808</v>
       </c>
       <c r="C17">
-        <v>0.69995</v>
+        <v>0.01314953435035937</v>
       </c>
       <c r="D17">
-        <v>0.05144</v>
+        <v>-1</v>
       </c>
       <c r="E17">
-        <v>0.2653865</v>
+        <v>-0.001176883909534299</v>
       </c>
       <c r="F17">
-        <v>0.0036736065</v>
+        <v>-0.9906928332508242</v>
       </c>
       <c r="G17">
-        <v>0.7139</v>
+        <v>0.7921650018950812</v>
       </c>
       <c r="H17">
-        <v>-8.475300000000001</v>
+        <v>-0.1058115376228517</v>
       </c>
       <c r="I17">
-        <v>120.7994</v>
+        <v>-0.3235570152882552</v>
       </c>
       <c r="J17">
-        <v>0.187375</v>
+        <v>-0.7519233726431591</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -950,31 +950,31 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.66766</v>
+        <v>0.2409023029159791</v>
       </c>
       <c r="C18">
-        <v>0.72206</v>
+        <v>0.102346099616951</v>
       </c>
       <c r="D18">
-        <v>0.05967799999999999</v>
+        <v>-0.9186802312871237</v>
       </c>
       <c r="E18">
-        <v>0.1777568</v>
+        <v>-0.3367420057843519</v>
       </c>
       <c r="F18">
-        <v>0.0273134458</v>
+        <v>-0.9304069020719923</v>
       </c>
       <c r="G18">
-        <v>0.71178</v>
+        <v>0.7826744282875655</v>
       </c>
       <c r="H18">
-        <v>-7.266560000000001</v>
+        <v>0.1617784281408459</v>
       </c>
       <c r="I18">
-        <v>113.35256</v>
+        <v>-0.8309388211907454</v>
       </c>
       <c r="J18">
-        <v>0.16272</v>
+        <v>-0.9054534004428205</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -982,31 +982,31 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.61897</v>
+        <v>-0.01422620451151424</v>
       </c>
       <c r="C19">
-        <v>0.8190000000000001</v>
+        <v>0.4934232157157008</v>
       </c>
       <c r="D19">
-        <v>0.092067</v>
+        <v>-0.5989586982886588</v>
       </c>
       <c r="E19">
-        <v>0.06510231</v>
+        <v>-0.7681359015365389</v>
       </c>
       <c r="F19">
-        <v>0.2340284851</v>
+        <v>-0.4032455929479771</v>
       </c>
       <c r="G19">
-        <v>0.313567</v>
+        <v>-1</v>
       </c>
       <c r="H19">
-        <v>-4.561730000000001</v>
+        <v>0.7605716897989543</v>
       </c>
       <c r="I19">
-        <v>129.07459</v>
+        <v>0.2402634570713253</v>
       </c>
       <c r="J19">
-        <v>0.224982</v>
+        <v>-0.5177394847720636</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1014,31 +1014,31 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.5774431818</v>
+        <v>-0.2318206827530194</v>
       </c>
       <c r="C20">
-        <v>0.7589886364</v>
+        <v>0.2513242781270737</v>
       </c>
       <c r="D20">
-        <v>0.05716590909</v>
+        <v>-0.9434778340774755</v>
       </c>
       <c r="E20">
-        <v>0.1047071936</v>
+        <v>-0.6164747912956963</v>
       </c>
       <c r="F20">
-        <v>0.07872443636</v>
+        <v>-0.7992994355869837</v>
       </c>
       <c r="G20">
-        <v>0.5278363636</v>
+        <v>-0.04078341175408529</v>
       </c>
       <c r="H20">
-        <v>-5.605227273</v>
+        <v>0.529563036526471</v>
       </c>
       <c r="I20">
-        <v>120.3989886</v>
+        <v>-0.3508385815950312</v>
       </c>
       <c r="J20">
-        <v>0.2017409091</v>
+        <v>-0.6624649089039416</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1046,31 +1046,31 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.7121967213</v>
+        <v>0.4742682349550682</v>
       </c>
       <c r="C21">
-        <v>0.7555245902</v>
+        <v>0.2373495597659345</v>
       </c>
       <c r="D21">
-        <v>0.07637868852000002</v>
+        <v>-0.7538227260926358</v>
       </c>
       <c r="E21">
-        <v>0.103287918</v>
+        <v>-0.6219096996622426</v>
       </c>
       <c r="F21">
-        <v>0.08744134672000001</v>
+        <v>-0.7770697134900569</v>
       </c>
       <c r="G21">
-        <v>0.4538</v>
+        <v>-0.3722209392911577</v>
       </c>
       <c r="H21">
-        <v>-5.368180328</v>
+        <v>0.5820403136058587</v>
       </c>
       <c r="I21">
-        <v>116.7554754</v>
+        <v>-0.5990851274111844</v>
       </c>
       <c r="J21">
-        <v>0.1907327869</v>
+        <v>-0.7310139783579295</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1078,31 +1078,31 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.5149199999999999</v>
+        <v>-0.5594330477612726</v>
       </c>
       <c r="C22">
-        <v>0.7112109999999999</v>
+        <v>0.05857886594091033</v>
       </c>
       <c r="D22">
-        <v>0.06920499999999999</v>
+        <v>-0.8246363569817616</v>
       </c>
       <c r="E22">
-        <v>0.160844054</v>
+        <v>-0.4015068934049625</v>
       </c>
       <c r="F22">
-        <v>0.0336264108</v>
+        <v>-0.9143076820775325</v>
       </c>
       <c r="G22">
-        <v>0.405435</v>
+        <v>-0.5887358414267692</v>
       </c>
       <c r="H22">
-        <v>-5.75354</v>
+        <v>0.4967296748934891</v>
       </c>
       <c r="I22">
-        <v>128.33083</v>
+        <v>0.1895882321493403</v>
       </c>
       <c r="J22">
-        <v>0.186029</v>
+        <v>-0.7603050971379206</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1110,31 +1110,31 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.44109375</v>
+        <v>-0.9462718436427466</v>
       </c>
       <c r="C23">
-        <v>0.87815625</v>
+        <v>0.7320724384227009</v>
       </c>
       <c r="D23">
-        <v>0.09768125</v>
+        <v>-0.543538752731938</v>
       </c>
       <c r="E23">
-        <v>0.059820665</v>
+        <v>-0.7883611887179912</v>
       </c>
       <c r="F23">
-        <v>0.78428125</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0.3623125</v>
+        <v>-0.7817817189692666</v>
       </c>
       <c r="H23">
-        <v>-5.84821875</v>
+        <v>0.4757697633566409</v>
       </c>
       <c r="I23">
-        <v>128.3230938</v>
+        <v>0.1890611351354643</v>
       </c>
       <c r="J23">
-        <v>0.22540625</v>
+        <v>-0.515097622500962</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1142,31 +1142,31 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5092894737</v>
+        <v>-0.588936185386046</v>
       </c>
       <c r="C24">
-        <v>0.7625223684</v>
+        <v>0.2655801242135793</v>
       </c>
       <c r="D24">
-        <v>0.09780526316</v>
+        <v>-0.5423145816359737</v>
       </c>
       <c r="E24">
-        <v>0.1065103447</v>
+        <v>-0.6095698878368208</v>
       </c>
       <c r="F24">
-        <v>0.4331298862</v>
+        <v>0.1044995406800511</v>
       </c>
       <c r="G24">
-        <v>0.3577723684</v>
+        <v>-0.8021064610153079</v>
       </c>
       <c r="H24">
-        <v>-6.932473684</v>
+        <v>0.2357382092853104</v>
       </c>
       <c r="I24">
-        <v>128.9400132</v>
+        <v>0.2310942228972905</v>
       </c>
       <c r="J24">
-        <v>0.223575</v>
+        <v>-0.52650106453739</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1174,31 +1174,31 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.7197926829000001</v>
+        <v>0.514069967250911</v>
       </c>
       <c r="C25">
-        <v>0.6114390244</v>
+        <v>-0.3439230577760566</v>
       </c>
       <c r="D25">
-        <v>0.254047561</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.1764303659</v>
+        <v>-0.3418213912030559</v>
       </c>
       <c r="F25">
-        <v>0.000536755</v>
+        <v>-0.9986923805932301</v>
       </c>
       <c r="G25">
-        <v>0.3855231707</v>
+        <v>-0.6778748421965506</v>
       </c>
       <c r="H25">
-        <v>-7.014317073</v>
+        <v>0.2176197804581887</v>
       </c>
       <c r="I25">
-        <v>129.0771829</v>
+        <v>0.2404401213053546</v>
       </c>
       <c r="J25">
-        <v>0.1909646341</v>
+        <v>-0.7295702344089832</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1206,31 +1206,31 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.6936458333</v>
+        <v>0.3770642841049017</v>
       </c>
       <c r="C26">
-        <v>0.7176458333</v>
+        <v>0.08453838780536493</v>
       </c>
       <c r="D26">
-        <v>0.06907291667</v>
+        <v>-0.8259401911461736</v>
       </c>
       <c r="E26">
-        <v>0.1391844792</v>
+        <v>-0.4844490677764226</v>
       </c>
       <c r="F26">
-        <v>0.006573627083</v>
+        <v>-0.9832972482358308</v>
       </c>
       <c r="G26">
-        <v>0.5339375</v>
+        <v>-0.01347054189856989</v>
       </c>
       <c r="H26">
-        <v>-5.22175</v>
+        <v>0.6144569511427045</v>
       </c>
       <c r="I26">
-        <v>110.87125</v>
+        <v>-1</v>
       </c>
       <c r="J26">
-        <v>0.1728833333</v>
+        <v>-0.8421649460081737</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1238,31 +1238,31 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.45916</v>
+        <v>-0.8516073253163561</v>
       </c>
       <c r="C27">
-        <v>0.82276</v>
+        <v>0.5085918762947319</v>
       </c>
       <c r="D27">
-        <v>0.070628</v>
+        <v>-0.8105894972004526</v>
       </c>
       <c r="E27">
-        <v>0.047298245</v>
+        <v>-0.8363139649281991</v>
       </c>
       <c r="F27">
-        <v>0.0292071162</v>
+        <v>-0.9255776948188875</v>
       </c>
       <c r="G27">
-        <v>0.523129</v>
+        <v>-0.06185679889707574</v>
       </c>
       <c r="H27">
-        <v>-6.54646</v>
+        <v>0.3211936326897471</v>
       </c>
       <c r="I27">
-        <v>131.65473</v>
+        <v>0.4160583032988878</v>
       </c>
       <c r="J27">
-        <v>0.297416</v>
+        <v>-0.06668314595070246</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1270,31 +1270,31 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.69808</v>
+        <v>0.4002986716969272</v>
       </c>
       <c r="C28">
-        <v>0.7035100000000001</v>
+        <v>0.02751135128157056</v>
       </c>
       <c r="D28">
-        <v>0.102141</v>
+        <v>-0.4995152229289215</v>
       </c>
       <c r="E28">
-        <v>0.24518015</v>
+        <v>-0.07855414641751057</v>
       </c>
       <c r="F28">
-        <v>0.0201809396</v>
+        <v>-0.9485961026181141</v>
       </c>
       <c r="G28">
-        <v>0.56718</v>
+        <v>0.1353456812843739</v>
       </c>
       <c r="H28">
-        <v>-4.913930000000001</v>
+        <v>0.6826019147092128</v>
       </c>
       <c r="I28">
-        <v>123.19329</v>
+        <v>-0.1604520967816256</v>
       </c>
       <c r="J28">
-        <v>0.283656</v>
+        <v>-0.1523685315732264</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1302,31 +1302,31 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.6282051282</v>
+        <v>0.03416452199428832</v>
       </c>
       <c r="C29">
-        <v>0.6592564103</v>
+        <v>-0.1510172874319982</v>
       </c>
       <c r="D29">
-        <v>0.05696923077</v>
+        <v>-0.9454193047612868</v>
       </c>
       <c r="E29">
-        <v>0.2730361538</v>
+        <v>0.02811634669261509</v>
       </c>
       <c r="F29">
-        <v>0.03346615154</v>
+        <v>-0.9147163726188058</v>
       </c>
       <c r="G29">
-        <v>0.7070128204999999</v>
+        <v>0.7613332641625701</v>
       </c>
       <c r="H29">
-        <v>-9.038256410000001</v>
+        <v>-0.2304384106297466</v>
       </c>
       <c r="I29">
-        <v>118.9654872</v>
+        <v>-0.4485085367835069</v>
       </c>
       <c r="J29">
-        <v>0.203125641</v>
+        <v>-0.6538419956164916</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1334,31 +1334,31 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.6690199999999999</v>
+        <v>0.2480285048075661</v>
       </c>
       <c r="C30">
-        <v>0.72728</v>
+        <v>0.1234047188250744</v>
       </c>
       <c r="D30">
-        <v>0.08294899999999999</v>
+        <v>-0.6889652109281352</v>
       </c>
       <c r="E30">
-        <v>0.12745301</v>
+        <v>-0.5293730135604281</v>
       </c>
       <c r="F30">
-        <v>0.005404269200000001</v>
+        <v>-0.9862793255656864</v>
       </c>
       <c r="G30">
-        <v>0.5104350000000001</v>
+        <v>-0.1186838467149074</v>
       </c>
       <c r="H30">
-        <v>-5.26508</v>
+        <v>0.6048645878416297</v>
       </c>
       <c r="I30">
-        <v>113.64654</v>
+        <v>-0.8109088348745086</v>
       </c>
       <c r="J30">
-        <v>0.165652</v>
+        <v>-0.8871954389133698</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1366,31 +1366,31 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.6044583333</v>
+        <v>-0.09026522413476901</v>
       </c>
       <c r="C31">
-        <v>0.4997888889</v>
+        <v>-0.7943440708085987</v>
       </c>
       <c r="D31">
-        <v>0.07998194444000001</v>
+        <v>-0.7182539062300839</v>
       </c>
       <c r="E31">
-        <v>0.5232716667</v>
+        <v>0.9863566508782506</v>
       </c>
       <c r="F31">
-        <v>0.007501033472</v>
+        <v>-0.9809321916450245</v>
       </c>
       <c r="G31">
-        <v>0.6309166667</v>
+        <v>0.4206747033664699</v>
       </c>
       <c r="H31">
-        <v>-11.79668056</v>
+        <v>-0.8410963055122327</v>
       </c>
       <c r="I31">
-        <v>119.781</v>
+        <v>-0.3929445180587052</v>
       </c>
       <c r="J31">
-        <v>0.2760361111</v>
+        <v>-0.1998186128811694</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1398,31 +1398,31 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.6731460673999999</v>
+        <v>0.2696484969477848</v>
       </c>
       <c r="C32">
-        <v>0.6031966292000001</v>
+        <v>-0.3771746788258001</v>
       </c>
       <c r="D32">
-        <v>0.07986067416000001</v>
+        <v>-0.7194510015349329</v>
       </c>
       <c r="E32">
-        <v>0.4414438202000001</v>
+        <v>0.6730088785644535</v>
       </c>
       <c r="F32">
-        <v>0.04983587191</v>
+        <v>-0.8729705797173057</v>
       </c>
       <c r="G32">
-        <v>0.7498651685</v>
+        <v>0.9531697561195878</v>
       </c>
       <c r="H32">
-        <v>-9.342393258</v>
+        <v>-0.2977680007349788</v>
       </c>
       <c r="I32">
-        <v>115.1337191</v>
+        <v>-0.709581611856632</v>
       </c>
       <c r="J32">
-        <v>0.1640573034</v>
+        <v>-0.8971258308553705</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1430,31 +1430,31 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.6731460673999999</v>
+        <v>0.2696484969477848</v>
       </c>
       <c r="C33">
-        <v>0.6031966292000001</v>
+        <v>-0.3771746788258001</v>
       </c>
       <c r="D33">
-        <v>0.07986067416000001</v>
+        <v>-0.7194510015349329</v>
       </c>
       <c r="E33">
-        <v>0.4414438202000001</v>
+        <v>0.6730088785644535</v>
       </c>
       <c r="F33">
-        <v>0.04983587191</v>
+        <v>-0.8729705797173057</v>
       </c>
       <c r="G33">
-        <v>0.7498651685</v>
+        <v>0.9531697561195878</v>
       </c>
       <c r="H33">
-        <v>-9.342393258</v>
+        <v>-0.2977680007349788</v>
       </c>
       <c r="I33">
-        <v>115.1337191</v>
+        <v>-0.709581611856632</v>
       </c>
       <c r="J33">
-        <v>0.1640573034</v>
+        <v>-0.8971258308553705</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1462,31 +1462,31 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.6102</v>
+        <v>-0.06017972700358953</v>
       </c>
       <c r="C34">
-        <v>0.448811</v>
+        <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.07245</v>
+        <v>-0.7926039887524238</v>
       </c>
       <c r="E34">
-        <v>0.5268345</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0.0339221048</v>
+        <v>-0.9135536080794917</v>
       </c>
       <c r="G34">
-        <v>0.6956</v>
+        <v>0.7102416542452996</v>
       </c>
       <c r="H34">
-        <v>-12.51447</v>
+        <v>-1</v>
       </c>
       <c r="I34">
-        <v>114.52613</v>
+        <v>-0.750978990450057</v>
       </c>
       <c r="J34">
-        <v>0.17493</v>
+        <v>-0.8294200749739962</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1494,31 +1494,31 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.65162</v>
+        <v>0.156855039429904</v>
       </c>
       <c r="C35">
-        <v>0.6957100000000001</v>
+        <v>-0.003955550983441469</v>
       </c>
       <c r="D35">
-        <v>0.076651</v>
+        <v>-0.7511346578028252</v>
       </c>
       <c r="E35">
-        <v>0.25764127</v>
+        <v>-0.03083610959327499</v>
       </c>
       <c r="F35">
-        <v>0.09751319900000001</v>
+        <v>-0.7513846406902835</v>
       </c>
       <c r="G35">
-        <v>0.74466</v>
+        <v>0.929867852917337</v>
       </c>
       <c r="H35">
-        <v>-8.43407</v>
+        <v>-0.09668407076609387</v>
       </c>
       <c r="I35">
-        <v>119.99181</v>
+        <v>-0.3785812232246126</v>
       </c>
       <c r="J35">
-        <v>0.202895</v>
+        <v>-0.655278228394498</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1526,31 +1526,31 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.64647</v>
+        <v>0.1298697896198484</v>
       </c>
       <c r="C36">
-        <v>0.580685</v>
+        <v>-0.4679915039363887</v>
       </c>
       <c r="D36">
-        <v>0.071727</v>
+        <v>-0.799740938592119</v>
       </c>
       <c r="E36">
-        <v>0.452712</v>
+        <v>0.7161587253389414</v>
       </c>
       <c r="F36">
-        <v>0.0412694878</v>
+        <v>-0.8948164322357236</v>
       </c>
       <c r="G36">
-        <v>0.69242</v>
+        <v>0.6960057938340265</v>
       </c>
       <c r="H36">
-        <v>-9.451779999999999</v>
+        <v>-0.3219839566450857</v>
       </c>
       <c r="I36">
-        <v>124.53307</v>
+        <v>-0.06916774047585861</v>
       </c>
       <c r="J36">
-        <v>0.151801</v>
+        <v>-0.9734474938739502</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1558,31 +1558,31 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.6180333333</v>
+        <v>-0.01913420157719603</v>
       </c>
       <c r="C37">
-        <v>0.647</v>
+        <v>-0.2004623214102015</v>
       </c>
       <c r="D37">
-        <v>0.08155</v>
+        <v>-0.702775159511446</v>
       </c>
       <c r="E37">
-        <v>0.1595106333</v>
+        <v>-0.4066130329867015</v>
       </c>
       <c r="F37">
-        <v>0.002643213667</v>
+        <v>-0.9933205241851445</v>
       </c>
       <c r="G37">
-        <v>0.5006633333</v>
+        <v>-0.1624285269434265</v>
       </c>
       <c r="H37">
-        <v>-7.078933332999999</v>
+        <v>0.2033150806872057</v>
       </c>
       <c r="I37">
-        <v>116.4767667</v>
+        <v>-0.6180746214149124</v>
       </c>
       <c r="J37">
-        <v>0.22072</v>
+        <v>-0.5442795366269475</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1590,31 +1590,63 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.66506</v>
+        <v>0.2270690874793684</v>
       </c>
       <c r="C38">
-        <v>0.78122</v>
+        <v>0.3192256721511866</v>
       </c>
       <c r="D38">
-        <v>0.082852</v>
+        <v>-0.6945227527811759</v>
       </c>
       <c r="E38">
-        <v>0.05432948</v>
+        <v>-0.778914957990108</v>
       </c>
       <c r="F38">
-        <v>0.0470131384</v>
+        <v>-0.8801688848907676</v>
       </c>
       <c r="G38">
-        <v>0.433144</v>
+        <v>-0.5126993354250449</v>
       </c>
       <c r="H38">
-        <v>-5.0312</v>
+        <v>0.6529880112062181</v>
       </c>
       <c r="I38">
-        <v>122.28176</v>
+        <v>-0.2497762425073606</v>
       </c>
       <c r="J38">
-        <v>0.188886</v>
+        <v>-0.7355895960088656</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.8253556551127872</v>
+      </c>
+      <c r="C39">
+        <v>-0.2916356536139544</v>
+      </c>
+      <c r="D39">
+        <v>-0.8625915051610537</v>
+      </c>
+      <c r="E39">
+        <v>-0.293392955260987</v>
+      </c>
+      <c r="F39">
+        <v>-0.6834516998939655</v>
+      </c>
+      <c r="G39">
+        <v>0.08962379837017798</v>
+      </c>
+      <c r="H39">
+        <v>0.005003540223319947</v>
+      </c>
+      <c r="I39">
+        <v>-0.7762632314029609</v>
+      </c>
+      <c r="J39">
+        <v>-0.7238908839602092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementação de global index
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>danceability</t>
   </si>
@@ -43,31 +43,139 @@
     <t>liveness</t>
   </si>
   <si>
-    <t>0.7791999999999999</t>
-  </si>
-  <si>
-    <t>0.6243999999999998</t>
-  </si>
-  <si>
-    <t>0.06536000000000002</t>
-  </si>
-  <si>
-    <t>0.189077</t>
-  </si>
-  <si>
-    <t>0.12415164966666664</t>
-  </si>
-  <si>
-    <t>0.5569666666666665</t>
-  </si>
-  <si>
-    <t>-7.974733333333334</t>
-  </si>
-  <si>
-    <t>114.15503333333335</t>
-  </si>
-  <si>
-    <t>0.1918766666666666</t>
+    <t>0.6650200000000001</t>
+  </si>
+  <si>
+    <t>0.7451333333333333</t>
+  </si>
+  <si>
+    <t>0.5243789473684211</t>
+  </si>
+  <si>
+    <t>0.7120000000000002</t>
+  </si>
+  <si>
+    <t>0.4865399999999999</t>
+  </si>
+  <si>
+    <t>0.7758200000000001</t>
+  </si>
+  <si>
+    <t>0.6195000000000002</t>
+  </si>
+  <si>
+    <t>0.8442105263157896</t>
+  </si>
+  <si>
+    <t>0.6897799999999998</t>
+  </si>
+  <si>
+    <t>0.80486</t>
+  </si>
+  <si>
+    <t>0.082386</t>
+  </si>
+  <si>
+    <t>0.07762666666666672</t>
+  </si>
+  <si>
+    <t>0.07373684210526313</t>
+  </si>
+  <si>
+    <t>0.055468</t>
+  </si>
+  <si>
+    <t>0.062732</t>
+  </si>
+  <si>
+    <t>0.06228746000000001</t>
+  </si>
+  <si>
+    <t>0.2659283333333333</t>
+  </si>
+  <si>
+    <t>0.05897290315789475</t>
+  </si>
+  <si>
+    <t>0.12148599000000004</t>
+  </si>
+  <si>
+    <t>0.0241865002</t>
+  </si>
+  <si>
+    <t>0.0470132104</t>
+  </si>
+  <si>
+    <t>0.04215750933333333</t>
+  </si>
+  <si>
+    <t>0.022514615263157896</t>
+  </si>
+  <si>
+    <t>0.13015698850000001</t>
+  </si>
+  <si>
+    <t>0.064895861</t>
+  </si>
+  <si>
+    <t>0.42242000000000013</t>
+  </si>
+  <si>
+    <t>0.6012666666666667</t>
+  </si>
+  <si>
+    <t>0.6208842105263159</t>
+  </si>
+  <si>
+    <t>0.471703</t>
+  </si>
+  <si>
+    <t>0.4537019999999999</t>
+  </si>
+  <si>
+    <t>-5.047700000000001</t>
+  </si>
+  <si>
+    <t>-7.482966666666668</t>
+  </si>
+  <si>
+    <t>-5.262652631578948</t>
+  </si>
+  <si>
+    <t>-6.581110000000003</t>
+  </si>
+  <si>
+    <t>-5.8405</t>
+  </si>
+  <si>
+    <t>121.88228</t>
+  </si>
+  <si>
+    <t>117.87040000000002</t>
+  </si>
+  <si>
+    <t>125.52905263157899</t>
+  </si>
+  <si>
+    <t>120.15134999999998</t>
+  </si>
+  <si>
+    <t>125.39779999999998</t>
+  </si>
+  <si>
+    <t>0.18999799999999997</t>
+  </si>
+  <si>
+    <t>0.14767333333333338</t>
+  </si>
+  <si>
+    <t>0.20245368421052637</t>
+  </si>
+  <si>
+    <t>0.17892300000000003</t>
+  </si>
+  <si>
+    <t>0.199264</t>
   </si>
 </sst>
 </file>
@@ -425,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1616,32 +1724,32 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>0.66506</v>
-      </c>
-      <c r="C38">
-        <v>0.78122</v>
-      </c>
-      <c r="D38">
-        <v>0.082852</v>
-      </c>
-      <c r="E38">
-        <v>0.05432948</v>
-      </c>
-      <c r="F38">
-        <v>0.0470131384</v>
-      </c>
-      <c r="G38">
-        <v>0.433144</v>
-      </c>
-      <c r="H38">
-        <v>-5.0312</v>
-      </c>
-      <c r="I38">
-        <v>122.28176</v>
-      </c>
-      <c r="J38">
-        <v>0.188886</v>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" t="s">
+        <v>44</v>
+      </c>
+      <c r="J38" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1649,31 +1757,127 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" t="s">
+        <v>40</v>
+      </c>
+      <c r="I39" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>11</v>
       </c>
-      <c r="E39" t="s">
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>12</v>
       </c>
-      <c r="F39" t="s">
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
         <v>13</v>
       </c>
-      <c r="G39" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" t="s">
-        <v>17</v>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J42" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>